<commit_message>
Updated Figure for Paths
</commit_message>
<xml_diff>
--- a/benchmarking/data/DWB/playground/benchmarking_other_playground_dynamic.xlsx
+++ b/benchmarking/data/DWB/playground/benchmarking_other_playground_dynamic.xlsx
@@ -494,16 +494,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.001</v>
+        <v>50.812</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3720153231867389</v>
+        <v>0.2593528856428975</v>
       </c>
       <c r="D2" t="n">
-        <v>36.66424560546875</v>
+        <v>35.37482070922852</v>
       </c>
       <c r="E2" t="n">
-        <v>1.905464887619019</v>
+        <v>1.826734662055969</v>
       </c>
     </row>
   </sheetData>
@@ -552,16 +552,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.805</v>
+        <v>51.002</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2639873652938197</v>
+        <v>0.2317258327108997</v>
       </c>
       <c r="D2" t="n">
-        <v>36.50013732910156</v>
+        <v>35.46334838867188</v>
       </c>
       <c r="E2" t="n">
-        <v>1.553720355033875</v>
+        <v>2.043991804122925</v>
       </c>
     </row>
   </sheetData>
@@ -610,16 +610,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.602</v>
+        <v>50.801</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2940065122151472</v>
+        <v>0.2081243245494995</v>
       </c>
       <c r="D2" t="n">
-        <v>36.5338134765625</v>
+        <v>35.7010612487793</v>
       </c>
       <c r="E2" t="n">
-        <v>1.933764338493347</v>
+        <v>1.96355926990509</v>
       </c>
     </row>
   </sheetData>
@@ -668,16 +668,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.804</v>
+        <v>51.018</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2038381086058867</v>
+        <v>0.28305833119626</v>
       </c>
       <c r="D2" t="n">
-        <v>35.93727493286133</v>
+        <v>35.61456298828125</v>
       </c>
       <c r="E2" t="n">
-        <v>1.903631448745728</v>
+        <v>2.108329296112061</v>
       </c>
     </row>
   </sheetData>
@@ -726,16 +726,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.199</v>
+        <v>51.41</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3789236602780925</v>
+        <v>0.1756432299417202</v>
       </c>
       <c r="D2" t="n">
-        <v>36.92699432373047</v>
+        <v>35.79704666137695</v>
       </c>
       <c r="E2" t="n">
-        <v>2.01080060005188</v>
+        <v>1.762745022773743</v>
       </c>
     </row>
   </sheetData>
@@ -784,16 +784,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.39700000000001</v>
+        <v>51.208</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1558123839829223</v>
+        <v>0.3612406802292721</v>
       </c>
       <c r="D2" t="n">
-        <v>36.75570297241211</v>
+        <v>35.70381164550781</v>
       </c>
       <c r="E2" t="n">
-        <v>1.66649854183197</v>
+        <v>1.866026639938354</v>
       </c>
     </row>
   </sheetData>
@@ -842,16 +842,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>82.001</v>
+        <v>51.013</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3582034966890335</v>
+        <v>0.3700479789610016</v>
       </c>
       <c r="D2" t="n">
-        <v>37.40874862670898</v>
+        <v>35.57451629638672</v>
       </c>
       <c r="E2" t="n">
-        <v>1.309641599655151</v>
+        <v>2.190979242324829</v>
       </c>
     </row>
   </sheetData>
@@ -900,16 +900,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.8</v>
+        <v>84.806</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3357544976121813</v>
+        <v>0.2400655657575073</v>
       </c>
       <c r="D2" t="n">
-        <v>36.52511978149414</v>
+        <v>36.01694488525391</v>
       </c>
       <c r="E2" t="n">
-        <v>2.27311110496521</v>
+        <v>1.417576432228088</v>
       </c>
     </row>
   </sheetData>
@@ -958,16 +958,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.80099999999999</v>
+        <v>51.027</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3622080092542908</v>
+        <v>0.3040378721061801</v>
       </c>
       <c r="D2" t="n">
-        <v>36.58796691894531</v>
+        <v>35.58433151245117</v>
       </c>
       <c r="E2" t="n">
-        <v>2.040711641311646</v>
+        <v>2.12936544418335</v>
       </c>
     </row>
   </sheetData>
@@ -1016,16 +1016,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.198</v>
+        <v>51.209</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2708498192121598</v>
+        <v>0.2428398027929857</v>
       </c>
       <c r="D2" t="n">
-        <v>36.59365844726562</v>
+        <v>35.55540084838867</v>
       </c>
       <c r="E2" t="n">
-        <v>1.983064532279968</v>
+        <v>1.886032342910767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>